<commit_message>
error handling for worksheet 1
</commit_message>
<xml_diff>
--- a/testdata/SampleAssessmentResult.xlsx
+++ b/testdata/SampleAssessmentResult.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvin Li\Desktop\UMel\SWEN90014 Project\swen90014-2019-rv-quoll\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14DE8B8D-4D5C-4F18-966F-457CF5157D10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760B3FBF-C3CD-4A12-8829-52C436BFFA8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="23152" windowHeight="11977" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23273" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AssessmentResult" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>student_id</t>
   </si>
@@ -132,6 +132,34 @@
   </si>
   <si>
     <t>Lists methods of evidence collection.</t>
+  </si>
+  <si>
+    <t>thr3e</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>f0ur</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>fiv3</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>s1x</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>s3ven</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>0ne</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>tw0</t>
+    <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -988,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1000,63 +1028,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>1.2</v>
       </c>
-      <c r="D1">
+      <c r="D2">
         <v>1.3</v>
       </c>
-      <c r="E1">
+      <c r="E2">
         <v>1.4</v>
       </c>
-      <c r="F1">
+      <c r="F2">
         <v>2.1</v>
       </c>
-      <c r="G1">
+      <c r="G2">
         <v>3.1</v>
       </c>
-      <c r="H1">
+      <c r="H2">
         <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>651</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1074,18 +1099,18 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1094,44 +1119,44 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1140,30 +1165,30 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1172,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -1183,13 +1208,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1209,13 +1234,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1235,25 +1260,25 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1261,22 +1286,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1287,16 +1312,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1305,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1313,16 +1338,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1339,7 +1364,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1365,19 +1390,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -1386,44 +1411,44 @@
         <v>3</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1432,27 +1457,27 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1464,44 +1489,44 @@
         <v>3</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1510,27 +1535,27 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1542,12 +1567,12 @@
         <v>3</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1556,10 +1581,10 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -1573,36 +1598,36 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1614,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>3</v>
@@ -1625,45 +1650,45 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>3</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26">
         <v>2</v>
@@ -1672,18 +1697,18 @@
         <v>3</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1698,12 +1723,12 @@
         <v>3</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1724,15 +1749,15 @@
         <v>3</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1747,7 +1772,7 @@
         <v>2</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1755,13 +1780,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1773,7 +1798,7 @@
         <v>2</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1781,13 +1806,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1796,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31">
         <v>3</v>
@@ -1807,7 +1832,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -1822,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>3</v>
@@ -1833,13 +1858,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1854,56 +1879,56 @@
         <v>3</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>2</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35">
         <v>2</v>
       </c>
       <c r="G35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1911,13 +1936,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1929,7 +1954,7 @@
         <v>2</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1937,65 +1962,65 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <v>2</v>
       </c>
       <c r="G37">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2007,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2015,7 +2040,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2024,16 +2049,16 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2041,27 +2066,53 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41">
+        <v>689</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A42">
         <v>690</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>2</v>
-      </c>
-      <c r="G41">
-        <v>3</v>
-      </c>
-      <c r="H41">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
         <v>0</v>
       </c>
     </row>
@@ -2077,7 +2128,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2273,5 +2324,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>